<commit_message>
Update product backlog template_with format example.xlsx
</commit_message>
<xml_diff>
--- a/product backlog template_with format example.xlsx
+++ b/product backlog template_with format example.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Story ID</t>
   </si>
@@ -22,19 +22,19 @@
     <t>Story Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Iteration (Sprint) number</t>
+  </si>
+  <si>
     <t>Acceptance Criteria</t>
   </si>
   <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Iteration (Sprint) number</t>
   </si>
   <si>
     <t>Date started (actual date)</t>
@@ -58,28 +58,365 @@
 3. List 3
 </t>
   </si>
+  <si>
+    <t>US01</t>
+  </si>
+  <si>
+    <t>User sign up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user  I want I can sign up the system with my telephone number/email together with some optional body characteristic. So that   coach or the system can better custom some classes for me.
+</t>
+  </si>
+  <si>
+    <t>Make sure the telephone number/ email is not used by other people
+Receive the user’s phone/email, name,password, gender(o), weight(o), height(o), age(o)
+Generate user entity with above information, store in the memory.</t>
+  </si>
+  <si>
+    <t>US02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User sign up legality </t>
+  </si>
+  <si>
+    <t>As a        staff of the gym
+  I want the user sign up procedure can make sure the phone/email is legal and password is encrypted 
+  So that   the system can be more safe</t>
+  </si>
+  <si>
+    <t>Make sure the phone/email is legal
+Make sure the stored password is encrypted once stored in memory</t>
+  </si>
+  <si>
+    <t>implementation of US01</t>
+  </si>
+  <si>
+    <t>US01G</t>
+  </si>
+  <si>
+    <t>User sign up GUI</t>
+  </si>
+  <si>
+    <t>As a       staff of gym
+  I want the sign up surface is clean and easy to use, where have some notice to introduce user to sign up
+  So that   it will not let people who want to register to give up because of the complicated interface</t>
+  </si>
+  <si>
+    <t>Make sure there is sign up link in sign in interface
+Make sure there is only email/phone, password, name , weight height shown
+Make sure the sign up procedure is done with continuously interface for good design</t>
+  </si>
+  <si>
+    <t>UL01</t>
+  </si>
+  <si>
+    <t>User log in</t>
+  </si>
+  <si>
+    <t>As a         user
+  I want I can sign in just with my phone/email and password
+  So that   i can save more time</t>
+  </si>
+  <si>
+    <t>Use email/phone as ID of the user
+Use password to make sure if the user have the authority to login
+If password wrong, show the message
+If user entity not exist, show the message.</t>
+  </si>
+  <si>
+    <t>UL01G</t>
+  </si>
+  <si>
+    <t>user login GUI</t>
+  </si>
+  <si>
+    <t>As a      staff
+  I want the GUI of login can be shown once user open the system and after the login procedure, it will jump to the home page
+  So that   i can have better user experiment</t>
+  </si>
+  <si>
+    <t>Once the system start, the login page will show out
+After the login procedure finish, it will change to the home page</t>
+  </si>
+  <si>
+    <t>MS01</t>
+  </si>
+  <si>
+    <t>Set up different membership</t>
+  </si>
+  <si>
+    <t>As a         user
+  I want to get higher membership when I recharge more money and get  
+  So that   I can enjoy some specific service</t>
+  </si>
+  <si>
+    <t>According to the money that they recharged, they can set to different membership
+Once a recharge procedure finish, check if the total recharged money is enough to upgrade membership
+For different membership, set up some rights for them to use</t>
+  </si>
+  <si>
+    <t>MS02</t>
+  </si>
+  <si>
+    <t>Set up bargain for recharge money</t>
+  </si>
+  <si>
+    <t>As a        staff
+  I want  the more money they recharge, the more bargain they can get
+  So that   user will be likely to deposit more money to the system</t>
+  </si>
+  <si>
+    <t>Set different bargain for different deposit level 
+Receive the user id, return current money and update membership</t>
+  </si>
+  <si>
+    <t>MS03</t>
+  </si>
+  <si>
+    <t>Set up 7 day free for video</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a        staff
+  I want  the new user can try to use the system without limitation for 7 days 
+  So that   they can adapt to the system and can increase user  retention</t>
+  </si>
+  <si>
+    <t>Set create time for user entity to compute the day to decide whether he can user the privilege
+Check the authority when the user update</t>
+  </si>
+  <si>
+    <t>MS04</t>
+  </si>
+  <si>
+    <t>Invitation code</t>
+  </si>
+  <si>
+    <t>As a        user
+I want that new users can register with old user’s invitation code.
+So that both the new and old users are able to earn some discount.</t>
+  </si>
+  <si>
+    <t>Generate and store the user’s invitation code and compare them when needed.
+Design the discount strategy.</t>
+  </si>
+  <si>
+    <t>MS05</t>
+  </si>
+  <si>
+    <t>Family membership</t>
+  </si>
+  <si>
+    <t>As a  user
+I want that users can register and purchase membership card in family unit.
+So that the whole family can share the membership and get some discount</t>
+  </si>
+  <si>
+    <t>Set different membership type and design different membership discount strategy</t>
+  </si>
+  <si>
+    <t>MS06</t>
+  </si>
+  <si>
+    <t>Family membership for kids</t>
+  </si>
+  <si>
+    <t>As a  user
+I want that kids can have discount or be free of charge in family membership.
+So that it will be more attractive to the family with kids.</t>
+  </si>
+  <si>
+    <t>Set different membership type and design different membership discount strategy.</t>
+  </si>
+  <si>
+    <t>Reliable data storage</t>
+  </si>
+  <si>
+    <t>As a  staff
+I want a reliable data storage  system during our developing process.
+So that it will be safer to store the user’s data.</t>
+  </si>
+  <si>
+    <t>Design and implement a well design data storage interface</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,12 +425,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -103,44 +620,330 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="36" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="36" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -189,7 +992,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,7 +1027,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,31 +1230,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G6:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.13888888888889" customWidth="1"/>
+    <col min="2" max="2" width="16.712962962963" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="19.8518518518519" customWidth="1"/>
+    <col min="7" max="7" width="17.1388888888889" customWidth="1"/>
+    <col min="8" max="8" width="24.8518518518519" customWidth="1"/>
+    <col min="9" max="9" width="26.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,19 +1262,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
@@ -480,16 +1283,188 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" ht="100.8" spans="3:6">
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" ht="75" customHeight="1" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="129.6" spans="1:7">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" ht="187.2" spans="1:6">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" ht="158.4" spans="1:6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" ht="144" spans="1:6">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" ht="216" spans="1:6">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" ht="129.6" spans="1:6">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" ht="144" spans="1:6">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" ht="100.8" spans="1:6">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" ht="115.2" spans="1:6">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" ht="100.8" spans="1:6">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" ht="100.8" spans="1:6">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>